<commit_message>
Created the basic game html view
</commit_message>
<xml_diff>
--- a/Project Documents/Timeline.xlsx
+++ b/Project Documents/Timeline.xlsx
@@ -554,7 +554,7 @@
   <dimension ref="A1:BG259"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="22.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1443,6 +1443,9 @@
       </c>
       <c r="E7" s="2">
         <v>3</v>
+      </c>
+      <c r="F7" s="5">
+        <v>42372</v>
       </c>
       <c r="I7" s="6" t="b">
         <f t="shared" ref="I7:X21" si="4">IF(AND(I$3&gt;=$F7, I$3&lt;=$F7+$G7-1), "ACTUAL", IF(AND(I$3&gt;=$D7, I$3&lt;=$D7+$E7-1), "PLANNED",  FALSE))</f>

</xml_diff>